<commit_message>
iRecorderQuestion 待测试 iRecorderScore 待测试
</commit_message>
<xml_diff>
--- a/doc/座席录音问题资源接口说明文档.xlsx
+++ b/doc/座席录音问题资源接口说明文档.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>REST接口说明</t>
   </si>
@@ -149,29 +149,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>TRQ_SCRSUB.SUBNO</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>subNO</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TRQ_SCRSUB.SUBDESC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>subDesc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>语音较低，造成用户反感，而要求提高声音</t>
-  </si>
-  <si>
-    <t>答案描述</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>JsonList</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -193,6 +170,10 @@
   </si>
   <si>
     <t>3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>questionCount</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -687,7 +668,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -720,7 +701,7 @@
         <v>26</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D3" s="6"/>
     </row>
@@ -743,7 +724,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>
@@ -763,7 +744,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -851,7 +832,7 @@
         <v>35</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>34</v>
@@ -862,31 +843,21 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="5" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>36</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>38</v>
-      </c>
+      <c r="A16" s="5"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="5"/>

</xml_diff>